<commit_message>
pop is entirely derived
</commit_message>
<xml_diff>
--- a/AmpersandData/FormalAmpersand/Atoms.xlsx
+++ b/AmpersandData/FormalAmpersand/Atoms.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Atoms" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>[Concept]</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Atom</t>
-  </si>
-  <si>
-    <t>pop</t>
   </si>
   <si>
     <t>repr</t>
@@ -411,7 +408,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C12" sqref="C12:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,21 +478,21 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
         <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -512,7 +509,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
@@ -526,9 +523,6 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
         <v>11</v>
       </c>
     </row>
@@ -539,9 +533,6 @@
       <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="C13" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -549,9 +540,6 @@
       </c>
       <c r="B14">
         <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -561,9 +549,6 @@
       <c r="B15">
         <v>2</v>
       </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -571,9 +556,6 @@
       </c>
       <c r="B16">
         <v>3</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The file Atoms.ifc was used in http://youtu.be/HVp0lsoBj18
To reproduce, compile Atoms.ifc with Ampersand [master:ddbd80c*].
</commit_message>
<xml_diff>
--- a/AmpersandData/FormalAmpersand/Atoms.xlsx
+++ b/AmpersandData/FormalAmpersand/Atoms.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956"/>
   </bookViews>
   <sheets>
     <sheet name="Atoms" sheetId="2" r:id="rId1"/>
     <sheet name="Concepts" sheetId="1" r:id="rId2"/>
     <sheet name="Relations" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>[Concept]</t>
   </si>
@@ -67,13 +68,16 @@
   </si>
   <si>
     <t>r</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,7 +123,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
   <a:themeElements>
     <a:clrScheme name="Kantoor">
       <a:dk1>
@@ -193,7 +197,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -228,7 +231,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -404,16 +406,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:C16"/>
+      <selection activeCell="B3" sqref="B3:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,18 +426,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -443,40 +445,40 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="H4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="H5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="H6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -490,12 +492,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
@@ -504,7 +506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>1</v>
       </c>
@@ -518,7 +520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -526,7 +528,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -534,7 +536,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>1</v>
       </c>
@@ -542,7 +544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>2</v>
       </c>
@@ -550,7 +552,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>3</v>
       </c>
@@ -564,28 +566,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
provide an example for ticket #202
Try running Atoms.ifc (which includes Atoms.adl and Atoms.xlsx).
This is the preferred implementation according to 2 relation-algebra specialists at the Braga conference, who regard the function repr as undesired in this program. Indeed. the program works as desired and has become much simpler. You can try it by adding a pair. The only thing that keeps it from running completely is Error! 501 Not Implemented: TgtConcept of interface: 'atoms' is scalar and can not have subinterfaces.
</commit_message>
<xml_diff>
--- a/AmpersandData/FormalAmpersand/Atoms.xlsx
+++ b/AmpersandData/FormalAmpersand/Atoms.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Atoms" sheetId="2" r:id="rId1"/>
-    <sheet name="Concepts" sheetId="1" r:id="rId2"/>
-    <sheet name="Relations" sheetId="3" r:id="rId3"/>
+    <sheet name="Concepts" sheetId="1" r:id="rId1"/>
+    <sheet name="Relations" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>[Concept]</t>
   </si>
@@ -42,15 +41,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>[Atom]</t>
-  </si>
-  <si>
-    <t>Atom</t>
-  </si>
-  <si>
-    <t>repr</t>
-  </si>
-  <si>
     <t>[Relation]</t>
   </si>
   <si>
@@ -66,26 +56,17 @@
     <t>r</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Identifier</t>
   </si>
   <si>
-    <t>Representation</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
+    <t>r1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,10 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -133,7 +113,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Kantoor">
       <a:dk1>
@@ -207,6 +187,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -241,6 +222,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -416,53 +398,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>20</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -471,130 +476,52 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
make AST compilable again.
</commit_message>
<xml_diff>
--- a/AmpersandData/FormalAmpersand/Atoms.xlsx
+++ b/AmpersandData/FormalAmpersand/Atoms.xlsx
@@ -47,9 +47,6 @@
     <t>Relation</t>
   </si>
   <si>
-    <t>source</t>
-  </si>
-  <si>
     <t>target</t>
   </si>
   <si>
@@ -60,6 +57,9 @@
   </si>
   <si>
     <t>r1</t>
+  </si>
+  <si>
+    <t>src</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -480,7 +480,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,10 +496,10 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -507,7 +507,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -518,10 +518,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
intermediate commit (will most likely not compile)
</commit_message>
<xml_diff>
--- a/AmpersandData/FormalAmpersand/Atoms.xlsx
+++ b/AmpersandData/FormalAmpersand/Atoms.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10411"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7293F1F4-B0D0-2942-B03B-029D996A77FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="14800" windowHeight="7960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concepts" sheetId="1" r:id="rId1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
   <si>
     <t>[Concept]</t>
   </si>
@@ -53,19 +54,22 @@
     <t>r</t>
   </si>
   <si>
-    <t>Identifier</t>
-  </si>
-  <si>
     <t>r1</t>
   </si>
   <si>
     <t>source</t>
+  </si>
+  <si>
+    <t>RelationName</t>
+  </si>
+  <si>
+    <t>ConceptName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -108,6 +112,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -115,7 +122,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -153,9 +160,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -188,9 +195,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -223,9 +247,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -398,16 +439,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -418,18 +459,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -437,7 +478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -448,7 +489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -459,7 +500,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -476,19 +517,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -496,18 +537,18 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -516,9 +557,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>

</xml_diff>